<commit_message>
fix get product va profile
</commit_message>
<xml_diff>
--- a/tool/products_fixed.xlsx
+++ b/tool/products_fixed.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Thức uống có gas phổ biến</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-09-15 14:54:30</t>
+    <t xml:space="preserve">9/15/2025 14:54</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.coca-cola.com/content/dam/brands/us/coca-cola/coca-cola-logo.png</t>
@@ -89,16 +89,101 @@
   </si>
   <si>
     <t xml:space="preserve">https://cdn.thtrue.vn/wp-content/uploads/2022/04/tra-xanh-0-do.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nước Cam Ép</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nước cam tươi nguyên chất</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bavifoods.com/thumbs/740x740x1/upload/product/cam-ep-5018.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cdn-i.vtcnews.vn/files/news/2019/01/22/-145625.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nước Chanh Tươi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nước chanh mát lạnh giải khát</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://media.baobinhphuoc.com.vn/upload/news/5_2023/img_8476_06413001052023.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://media.vov.vn/sites/default/files/styles/large/public/2023-06/nuoc_chanh_5.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://suckhoedoisong.qltns.mediacdn.vn/324455921873985536/2022/4/18/uong-nuoc-chanh-moi-ngay-co-tot-khong-va-uong-khi-nao-chanh1-1592466583-666-width1024height768-16502694973802093569436.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nước Dừa Xiêm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nước dừa xiêm ngọt thanh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chi-em-thi-nhau-lung-mua-dua-xiem-ve-uong-sau-tiem-phong-cua-hang-moi-ngay-ban-5000-qua-1-1631524190-570-width650height431.jpg (650×431)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medium_20200513_094458_574364_nuoc_dua_max_1800x1800_jpg_095dc5e7ad.jpg (750×563)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coconut-water-benefits-17218412875751213756362.jpg (800×562)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sữa Tươi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sữa tươi tiệt trùng nguyên chất</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://file.hstatic.net/1000199715/file/uong-sua-sau-sinh-1_90f6b928e6084e7e87c4e7a89e1b1be3_grande.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">khi_nao_nen_cho_be_uong_sua_1_4401cf044a.jpg (800×600)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sữa Đậu Nành</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thức uống từ đậu nành bổ dưỡng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://suckhoedoisong.qltns.mediacdn.vn/324455921873985536/2025/2/21/dau-nanh-1-1740125251401155246723.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glass-soy-milk_20dc83bb32164c49bd11a7d7b60b717b_grande.jpg (600×377)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">may-lam-sua-dau-nanh-1-1412734006024.jpg (500×455)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trà Sữa Trân Châu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trà sữa kèm trân châu dai ngon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://baothainguyen.vn/file/e7837c027f6ecd14017ffa4e5f2a0e34/032023/1-boba-tea-recipe-using-fresh-tapioca-pearls-1024x1024-1677809524112848165864_20230305161118.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.cet.edu.vn/wp-content/uploads/2018/04/tra-sua-tu-lam.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +213,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -171,7 +262,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -182,6 +273,26 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -376,20 +487,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="109.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="65.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="53.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="65.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="53.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,124 +532,281 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="4" t="n">
         <v>12000</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="4" t="n">
         <v>11000</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="4" t="n">
         <v>10000</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="4" t="n">
         <v>120</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>15000</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>20000</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>70</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>18000</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>35000</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="https://upload.wikimedia.org/wikipedia/commons/2/27/Coca_Cola_Flasche_-_Original_Taste.jpg"/>
-    <hyperlink ref="I2" r:id="rId2" display="https://product.hstatic.net/200000534989/product/dsc08341-enhanced-nr_1_e6d5d0a13c8f42c2bd7cea59e03ce199_master.jpg"/>
+    <hyperlink ref="G5" r:id="rId1" display="https://bavifoods.com/thumbs/740x740x1/upload/product/cam-ep-5018.jpg"/>
+    <hyperlink ref="H5" r:id="rId2" display="https://bavifoods.com/thumbs/740x740x1/upload/product/cam-ep-5018.jpg"/>
+    <hyperlink ref="I5" r:id="rId3" display="https://cdn-i.vtcnews.vn/files/news/2019/01/22/-145625.jpg"/>
+    <hyperlink ref="G6" r:id="rId4" display="https://media.baobinhphuoc.com.vn/upload/news/5_2023/img_8476_06413001052023.jpeg"/>
+    <hyperlink ref="H6" r:id="rId5" display="https://media.vov.vn/sites/default/files/styles/large/public/2023-06/nuoc_chanh_5.jpg"/>
+    <hyperlink ref="I6" r:id="rId6" display="https://suckhoedoisong.qltns.mediacdn.vn/324455921873985536/2022/4/18/uong-nuoc-chanh-moi-ngay-co-tot-khong-va-uong-khi-nao-chanh1-1592466583-666-width1024height768-16502694973802093569436.jpg"/>
+    <hyperlink ref="G7" r:id="rId7" display="Chi-em-thi-nhau-lung-mua-dua-xiem-ve-uong-sau-tiem-phong-cua-hang-moi-ngay-ban-5000-qua-1-1631524190-570-width650height431.jpg (650×431)"/>
+    <hyperlink ref="H7" r:id="rId8" display="medium_20200513_094458_574364_nuoc_dua_max_1800x1800_jpg_095dc5e7ad.jpg (750×563)"/>
+    <hyperlink ref="I7" r:id="rId9" display="coconut-water-benefits-17218412875751213756362.jpg (800×562)"/>
+    <hyperlink ref="G8" r:id="rId10" display="https://file.hstatic.net/1000199715/file/uong-sua-sau-sinh-1_90f6b928e6084e7e87c4e7a89e1b1be3_grande.jpg"/>
+    <hyperlink ref="H8" r:id="rId11" display="khi_nao_nen_cho_be_uong_sua_1_4401cf044a.jpg (800×600)"/>
+    <hyperlink ref="G9" r:id="rId12" display="https://suckhoedoisong.qltns.mediacdn.vn/324455921873985536/2025/2/21/dau-nanh-1-1740125251401155246723.jpg"/>
+    <hyperlink ref="H9" r:id="rId13" display="glass-soy-milk_20dc83bb32164c49bd11a7d7b60b717b_grande.jpg (600×377)"/>
+    <hyperlink ref="I9" r:id="rId14" display="may-lam-sua-dau-nanh-1-1412734006024.jpg (500×455)"/>
+    <hyperlink ref="G10" r:id="rId15" display="https://baothainguyen.vn/file/e7837c027f6ecd14017ffa4e5f2a0e34/032023/1-boba-tea-recipe-using-fresh-tapioca-pearls-1024x1024-1677809524112848165864_20230305161118.jpeg"/>
+    <hyperlink ref="H10" r:id="rId16" display="https://www.cet.edu.vn/wp-content/uploads/2018/04/tra-sua-tu-lam.jpg"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
them cot public_id, chuc nang nhan don hang cuar shipper, xoa san pham cua admin
</commit_message>
<xml_diff>
--- a/tool/products_fixed.xlsx
+++ b/tool/products_fixed.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -49,141 +49,143 @@
     <t xml:space="preserve">ProductImageURL3</t>
   </si>
   <si>
-    <t xml:space="preserve">Coca Cola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thức uống có gas phổ biến</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9/15/2025 14:54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.coca-cola.com/content/dam/brands/us/coca-cola/coca-cola-logo.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/2/27/Coca_Cola_Flasche_-_Original_Taste.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://product.hstatic.net/200000534989/product/dsc08341-enhanced-nr_1_e6d5d0a13c8f42c2bd7cea59e03ce199_master.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pepsi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nước ngọt có gas vị cola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.pepsi.com/en-us/uploads/images/twil-can.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.oreo.com/images/hero/oreo-original.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://cdn.lottemart.vn/media/catalog/product/cache/9b5f86ccf0bb6d794da3fb554015eb8c/s/t/sting_dau_330ml.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trà Xanh 0 Độ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trà xanh đóng chai giải khát</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://cdn.thtrue.vn/wp-content/uploads/2022/04/tra-xanh-0-do.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nước Cam Ép</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nước cam tươi nguyên chất</t>
+    <t xml:space="preserve">Trà Đào Cam Sả</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trà đào cam sả mát lạnh</t>
   </si>
   <si>
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">https://bavifoods.com/thumbs/740x740x1/upload/product/cam-ep-5018.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://cdn-i.vtcnews.vn/files/news/2019/01/22/-145625.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nước Chanh Tươi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nước chanh mát lạnh giải khát</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://media.baobinhphuoc.com.vn/upload/news/5_2023/img_8476_06413001052023.jpeg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://media.vov.vn/sites/default/files/styles/large/public/2023-06/nuoc_chanh_5.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://suckhoedoisong.qltns.mediacdn.vn/324455921873985536/2022/4/18/uong-nuoc-chanh-moi-ngay-co-tot-khong-va-uong-khi-nao-chanh1-1592466583-666-width1024height768-16502694973802093569436.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nước Dừa Xiêm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nước dừa xiêm ngọt thanh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chi-em-thi-nhau-lung-mua-dua-xiem-ve-uong-sau-tiem-phong-cua-hang-moi-ngay-ban-5000-qua-1-1631524190-570-width650height431.jpg (650×431)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medium_20200513_094458_574364_nuoc_dua_max_1800x1800_jpg_095dc5e7ad.jpg (750×563)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coconut-water-benefits-17218412875751213756362.jpg (800×562)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sữa Tươi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sữa tươi tiệt trùng nguyên chất</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://file.hstatic.net/1000199715/file/uong-sua-sau-sinh-1_90f6b928e6084e7e87c4e7a89e1b1be3_grande.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">khi_nao_nen_cho_be_uong_sua_1_4401cf044a.jpg (800×600)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sữa Đậu Nành</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thức uống từ đậu nành bổ dưỡng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://suckhoedoisong.qltns.mediacdn.vn/324455921873985536/2025/2/21/dau-nanh-1-1740125251401155246723.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glass-soy-milk_20dc83bb32164c49bd11a7d7b60b717b_grande.jpg (600×377)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">may-lam-sua-dau-nanh-1-1412734006024.jpg (500×455)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trà Sữa Trân Châu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trà sữa kèm trân châu dai ngon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://baothainguyen.vn/file/e7837c027f6ecd14017ffa4e5f2a0e34/032023/1-boba-tea-recipe-using-fresh-tapioca-pearls-1024x1024-1677809524112848165864_20230305161118.jpeg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.cet.edu.vn/wp-content/uploads/2018/04/tra-sua-tu-lam.jpg</t>
+    <t xml:space="preserve">https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRXtYkBiYM_AEWth56eq5VeEwFGlnh_cYm7cw&amp;s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cà Phê Đen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cà phê đen nguyên chất</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://billballcoffeetea.com/upload/product/img3589-3619-8202.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cà Phê Sữa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cà phê sữa đá truyền thống</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://vcdn1-suckhoe.vnecdn.net/2023/02/01/iced-coffee-table-jpeg-1675223-7169-5352-1675223880.jpg?w=1200&amp;h=0&amp;q=100&amp;dpr=1&amp;fit=crop&amp;s=ExRy7hbEHS2p2f2oOgWCjA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinh Tố Bơ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinh tố bơ béo ngậy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQie4Hw_GApMLyRn34hNhlXh46_33_56ZcfMA&amp;s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burger Bò Phô Mai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bánh burger bò kèm phô mai tan chảy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cdn.tgdd.vn/2020/07/CookProductThumb/59-620x620-3.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burger Gà Giòn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bánh burger gà chiên giòn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://product.hstatic.net/200000848723/product/combo_2_burger_e7394736b32d499e8b9482c04030f5f5_master.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khoai Tây Chiên</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khoai tây chiên giòn, ăn kèm sốt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.bluestone.com.vn/blogs/vao-bep/chien-khoai-tay-bang-noi-chien-khong-dau?srsltid=AfmBOoqJ8H9yAh7LTcp--k4VJ6EP2X2OuqePxFBm3Y8K1ygpG_FpQDcN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gà Rán 2 Miếng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gà rán giòn rụm, hương vị đặc trưng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.giftpop.vn/brand/LOTTERIA/1PEMP2010312501_BASIC_origin.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotdog Xúc Xích</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bánh mì kẹp xúc xích và tương cà</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cdn.tgdd.vn/Files/2020/03/02/1239549/2-cong-thuc-lam-banh-hotdog-xuc-xich-hotdog-pho-mai-han-quoc-gay-nghien-14-760x367.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pizza Phô Mai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pizza nhỏ phủ phô mai mozzarella</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://checkinvietnam.vtc.vn/media/20211221/files/pizza-xuc-xich-pho-mai-vuong.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pizza Hải Sản</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pizza hải sản tươi ngon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://i.ytimg.com/vi/ng3vo1RmeyQ/maxresdefault.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandwich Thịt Nguội</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bánh sandwich kẹp thịt nguội và rau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://storage.googleapis.com/onelife-public/blog.onelife.vn/2021/10/cach-lam-banh-mi-sandwich-trung-jambon-mon-an-sang-349515833958.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mì Ý Sốt Bò Bằm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mì Ý sốt cà chua bò bằm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cdnv2.tgdd.vn/bhx-static/bhx/Products/Images/7259/332717/bhx/frame-3475095-2-1_202412022211137044.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salad Rau Trộn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salad rau củ tươi mát</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cdn.tgdd.vn/Files/2022/03/07/1418886/9-cach-lam-salad-tron-mayonnaise-giam-can-tai-nha-hieu-qua-202203071357195806.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,12 +214,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -262,7 +258,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -283,15 +279,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -487,10 +479,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -540,13 +532,13 @@
         <v>10</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>12000</v>
+        <v>30000</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>11</v>
@@ -554,54 +546,46 @@
       <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>11000</v>
+        <v>20000</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>80</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>10000</v>
+        <v>25000</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>40</v>
@@ -610,203 +594,302 @@
         <v>11</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>40000</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C6" s="4" t="n">
+        <v>45000</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="4" t="n">
-        <v>15000</v>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>35</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>12000</v>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>90</v>
-      </c>
-      <c r="E6" s="4" t="n">
-        <v>28</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>25</v>
+      <c r="F7" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>18000</v>
+        <v>25000</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E8" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="6"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>12000</v>
+        <v>60000</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E9" s="4" t="n">
-        <v>22</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>70</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>70000</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>85000</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>35000</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C14" s="4" t="n">
+        <v>65000</v>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>45</v>
+      </c>
+      <c r="E14" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="4" t="n">
-        <v>35000</v>
-      </c>
-      <c r="D10" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="E10" s="4" t="n">
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="C15" s="4" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D15" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="I10" s="6"/>
+      <c r="E15" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" display="https://bavifoods.com/thumbs/740x740x1/upload/product/cam-ep-5018.jpg"/>
-    <hyperlink ref="H5" r:id="rId2" display="https://bavifoods.com/thumbs/740x740x1/upload/product/cam-ep-5018.jpg"/>
-    <hyperlink ref="I5" r:id="rId3" display="https://cdn-i.vtcnews.vn/files/news/2019/01/22/-145625.jpg"/>
-    <hyperlink ref="G6" r:id="rId4" display="https://media.baobinhphuoc.com.vn/upload/news/5_2023/img_8476_06413001052023.jpeg"/>
-    <hyperlink ref="H6" r:id="rId5" display="https://media.vov.vn/sites/default/files/styles/large/public/2023-06/nuoc_chanh_5.jpg"/>
-    <hyperlink ref="I6" r:id="rId6" display="https://suckhoedoisong.qltns.mediacdn.vn/324455921873985536/2022/4/18/uong-nuoc-chanh-moi-ngay-co-tot-khong-va-uong-khi-nao-chanh1-1592466583-666-width1024height768-16502694973802093569436.jpg"/>
-    <hyperlink ref="G7" r:id="rId7" display="Chi-em-thi-nhau-lung-mua-dua-xiem-ve-uong-sau-tiem-phong-cua-hang-moi-ngay-ban-5000-qua-1-1631524190-570-width650height431.jpg (650×431)"/>
-    <hyperlink ref="H7" r:id="rId8" display="medium_20200513_094458_574364_nuoc_dua_max_1800x1800_jpg_095dc5e7ad.jpg (750×563)"/>
-    <hyperlink ref="I7" r:id="rId9" display="coconut-water-benefits-17218412875751213756362.jpg (800×562)"/>
-    <hyperlink ref="G8" r:id="rId10" display="https://file.hstatic.net/1000199715/file/uong-sua-sau-sinh-1_90f6b928e6084e7e87c4e7a89e1b1be3_grande.jpg"/>
-    <hyperlink ref="H8" r:id="rId11" display="khi_nao_nen_cho_be_uong_sua_1_4401cf044a.jpg (800×600)"/>
-    <hyperlink ref="G9" r:id="rId12" display="https://suckhoedoisong.qltns.mediacdn.vn/324455921873985536/2025/2/21/dau-nanh-1-1740125251401155246723.jpg"/>
-    <hyperlink ref="H9" r:id="rId13" display="glass-soy-milk_20dc83bb32164c49bd11a7d7b60b717b_grande.jpg (600×377)"/>
-    <hyperlink ref="I9" r:id="rId14" display="may-lam-sua-dau-nanh-1-1412734006024.jpg (500×455)"/>
-    <hyperlink ref="G10" r:id="rId15" display="https://baothainguyen.vn/file/e7837c027f6ecd14017ffa4e5f2a0e34/032023/1-boba-tea-recipe-using-fresh-tapioca-pearls-1024x1024-1677809524112848165864_20230305161118.jpeg"/>
-    <hyperlink ref="H10" r:id="rId16" display="https://www.cet.edu.vn/wp-content/uploads/2018/04/tra-sua-tu-lam.jpg"/>
+    <hyperlink ref="G2" r:id="rId1" display="https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRXtYkBiYM_AEWth56eq5VeEwFGlnh_cYm7cw&amp;s"/>
+    <hyperlink ref="G3" r:id="rId2" display="https://billballcoffeetea.com/upload/product/img3589-3619-8202.jpg"/>
+    <hyperlink ref="G4" r:id="rId3" display="https://vcdn1-suckhoe.vnecdn.net/2023/02/01/iced-coffee-table-jpeg-1675223-7169-5352-1675223880.jpg?w=1200&amp;h=0&amp;q=100&amp;dpr=1&amp;fit=crop&amp;s=ExRy7hbEHS2p2f2oOgWCjA"/>
+    <hyperlink ref="G5" r:id="rId4" display="https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQie4Hw_GApMLyRn34hNhlXh46_33_56ZcfMA&amp;s"/>
+    <hyperlink ref="G6" r:id="rId5" display="https://cdn.tgdd.vn/2020/07/CookProductThumb/59-620x620-3.jpg"/>
+    <hyperlink ref="G7" r:id="rId6" display="https://product.hstatic.net/200000848723/product/combo_2_burger_e7394736b32d499e8b9482c04030f5f5_master.jpg"/>
+    <hyperlink ref="G8" r:id="rId7" display="https://www.bluestone.com.vn/blogs/vao-bep/chien-khoai-tay-bang-noi-chien-khong-dau?srsltid=AfmBOoqJ8H9yAh7LTcp--k4VJ6EP2X2OuqePxFBm3Y8K1ygpG_FpQDcN"/>
+    <hyperlink ref="G9" r:id="rId8" display="https://img.giftpop.vn/brand/LOTTERIA/1PEMP2010312501_BASIC_origin.jpg"/>
+    <hyperlink ref="G10" r:id="rId9" display="https://cdn.tgdd.vn/Files/2020/03/02/1239549/2-cong-thuc-lam-banh-hotdog-xuc-xich-hotdog-pho-mai-han-quoc-gay-nghien-14-760x367.png"/>
+    <hyperlink ref="G11" r:id="rId10" display="https://checkinvietnam.vtc.vn/media/20211221/files/pizza-xuc-xich-pho-mai-vuong.jpg"/>
+    <hyperlink ref="G12" r:id="rId11" display="https://i.ytimg.com/vi/ng3vo1RmeyQ/maxresdefault.jpg"/>
+    <hyperlink ref="G13" r:id="rId12" display="https://storage.googleapis.com/onelife-public/blog.onelife.vn/2021/10/cach-lam-banh-mi-sandwich-trung-jambon-mon-an-sang-349515833958.jpg"/>
+    <hyperlink ref="G14" r:id="rId13" display="https://cdnv2.tgdd.vn/bhx-static/bhx/Products/Images/7259/332717/bhx/frame-3475095-2-1_202412022211137044.jpg"/>
+    <hyperlink ref="G15" r:id="rId14" display="https://cdn.tgdd.vn/Files/2022/03/07/1418886/9-cach-lam-salad-tron-mayonnaise-giam-can-tai-nha-hieu-qua-202203071357195806.jpg"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>